<commit_message>
23041305 homework 1.1 finished
</commit_message>
<xml_diff>
--- a/task2.xlsx
+++ b/task2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,140 +434,45 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Student_id</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>№</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>sku</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>volume</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>price</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>priceoforder</t>
+          <t>Student_name</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B2" t="n">
-        <v>5</v>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>205</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
-          <t>Киви</t>
+          <t>Ирина</t>
         </is>
-      </c>
-      <c r="D2" t="n">
-        <v>23</v>
-      </c>
-      <c r="E2" t="n">
-        <v>60</v>
-      </c>
-      <c r="F2" t="n">
-        <v>1380</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B3" t="n">
-        <v>7</v>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>206</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
-          <t>Киви</t>
+          <t>Ксения</t>
         </is>
-      </c>
-      <c r="D3" t="n">
-        <v>60</v>
-      </c>
-      <c r="E3" t="n">
-        <v>60</v>
-      </c>
-      <c r="F3" t="n">
-        <v>3600</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B4" t="n">
-        <v>25</v>
-      </c>
-      <c r="C4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>207</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
-          <t>Киви</t>
+          <t>Жанна</t>
         </is>
-      </c>
-      <c r="D4" t="n">
-        <v>45</v>
-      </c>
-      <c r="E4" t="n">
-        <v>60</v>
-      </c>
-      <c r="F4" t="n">
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B5" t="n">
-        <v>28</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Киви</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>23</v>
-      </c>
-      <c r="E5" t="n">
-        <v>60</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1380</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B6" t="n">
-        <v>30</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Киви</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>60</v>
-      </c>
-      <c r="E6" t="n">
-        <v>60</v>
-      </c>
-      <c r="F6" t="n">
-        <v>3600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>